<commit_message>
minor changes to survey final screen. Added docs.
</commit_message>
<xml_diff>
--- a/docs/Roles Timeline.xlsx
+++ b/docs/Roles Timeline.xlsx
@@ -1,22 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="192" yWindow="24" windowWidth="12420" windowHeight="6096"/>
+    <workbookView xWindow="200" yWindow="20" windowWidth="16380" windowHeight="11100"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$D$9:$K$19</definedName>
+  </definedNames>
+  <calcPr calcId="145621" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="20">
   <si>
     <t>Pressure</t>
   </si>
@@ -34,9 +42,6 @@
   </si>
   <si>
     <t>1/3</t>
-  </si>
-  <si>
-    <t>t</t>
   </si>
   <si>
     <t>SP</t>
@@ -85,10 +90,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -112,16 +123,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -130,7 +141,7 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -145,11 +156,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -455,18 +466,18 @@
   <dimension ref="D3:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9:K19"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="4" max="4" width="15.5546875" customWidth="1"/>
-    <col min="5" max="7" width="5.88671875" customWidth="1"/>
-    <col min="8" max="8" width="1.21875" customWidth="1"/>
-    <col min="9" max="11" width="5.88671875" customWidth="1"/>
+    <col min="4" max="4" width="15.5" customWidth="1"/>
+    <col min="5" max="7" width="5.83203125" customWidth="1"/>
+    <col min="8" max="8" width="1.1640625" customWidth="1"/>
+    <col min="9" max="11" width="5.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="4:11">
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
         <v>2</v>
@@ -475,7 +486,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="4:11">
       <c r="D4" s="1" t="s">
         <v>0</v>
       </c>
@@ -486,7 +497,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="4:11">
       <c r="D5" s="1" t="s">
         <v>1</v>
       </c>
@@ -497,166 +508,163 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="E9" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
+    <row r="9" spans="4:11">
+      <c r="E9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
       <c r="H9" s="3"/>
-      <c r="I9" s="4" t="s">
+      <c r="I9" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-    </row>
-    <row r="10" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D10" t="s">
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+    </row>
+    <row r="10" spans="4:11">
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" t="s">
         <v>6</v>
       </c>
-      <c r="E10" t="s">
+      <c r="G10" t="s">
         <v>8</v>
       </c>
-      <c r="F10" t="s">
+      <c r="I10" t="s">
         <v>7</v>
       </c>
-      <c r="G10" t="s">
+      <c r="J10" t="s">
+        <v>6</v>
+      </c>
+      <c r="K10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="4:11">
+      <c r="D11" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="I10" t="s">
-        <v>8</v>
-      </c>
-      <c r="J10" t="s">
-        <v>7</v>
-      </c>
-      <c r="K10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D11" s="5" t="s">
-        <v>10</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" spans="4:11" ht="28">
+      <c r="D12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="K11" s="1"/>
-    </row>
-    <row r="12" spans="4:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D12" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D13" s="5" t="s">
-        <v>16</v>
+    <row r="13" spans="4:11">
+      <c r="D13" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D14" s="5" t="s">
-        <v>14</v>
+    <row r="14" spans="4:11">
+      <c r="D14" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J14" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="K14" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D15" s="5" t="s">
-        <v>17</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="4:11">
+      <c r="D15" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J15" s="1"/>
       <c r="K15" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="4:11" ht="28">
+      <c r="D16" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="4:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D16" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J16" s="1"/>
       <c r="K16" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4">
       <c r="D18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="4:4">
+      <c r="D19" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D19" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -664,7 +672,14 @@
     <mergeCell ref="E9:G9"/>
     <mergeCell ref="I9:K9"/>
   </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -674,9 +689,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -686,8 +706,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>